<commit_message>
most of yuval fill db
</commit_message>
<xml_diff>
--- a/backend/datasets/raw_ingredients.xlsx
+++ b/backend/datasets/raw_ingredients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tamar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Documents\University\Computer Science\courses\99_misc\hackathon\meal_planner_huji_hackathon\backend\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AB2B02-B2BC-4D04-88DC-4EE5DB227736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036ECDC8-B6F0-4CE4-A11C-ED2590F61454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="groceries" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>chicken</t>
   </si>
@@ -34,30 +34,15 @@
     <t>sugar</t>
   </si>
   <si>
-    <t>soda</t>
-  </si>
-  <si>
-    <t>fish</t>
-  </si>
-  <si>
     <t>white wine</t>
   </si>
   <si>
-    <t>meat</t>
-  </si>
-  <si>
     <t>onions</t>
   </si>
   <si>
     <t>margarine</t>
   </si>
   <si>
-    <t>salt</t>
-  </si>
-  <si>
-    <t>oil</t>
-  </si>
-  <si>
     <t>baking powder</t>
   </si>
   <si>
@@ -76,12 +61,6 @@
     <t>rice</t>
   </si>
   <si>
-    <t>grocery</t>
-  </si>
-  <si>
-    <t>water</t>
-  </si>
-  <si>
     <t>cocoa</t>
   </si>
   <si>
@@ -100,21 +79,12 @@
     <t>nuts</t>
   </si>
   <si>
-    <t>soy</t>
-  </si>
-  <si>
-    <t>wheat</t>
-  </si>
-  <si>
     <t>walnuts</t>
   </si>
   <si>
     <t>pecans</t>
   </si>
   <si>
-    <t>onion</t>
-  </si>
-  <si>
     <t>cream cheese</t>
   </si>
   <si>
@@ -136,12 +106,6 @@
     <t>chicken broth</t>
   </si>
   <si>
-    <t>unsalted butter</t>
-  </si>
-  <si>
-    <t>pepper</t>
-  </si>
-  <si>
     <t>cinnamon</t>
   </si>
   <si>
@@ -160,9 +124,6 @@
     <t>cheddar cheese</t>
   </si>
   <si>
-    <t>lemon juice</t>
-  </si>
-  <si>
     <t>potatoes</t>
   </si>
   <si>
@@ -172,18 +133,9 @@
     <t>parmesan cheese</t>
   </si>
   <si>
-    <t>black pepper</t>
-  </si>
-  <si>
-    <t>vegetable oil</t>
-  </si>
-  <si>
     <t>vanilla</t>
   </si>
   <si>
-    <t>olive oil</t>
-  </si>
-  <si>
     <t>celery</t>
   </si>
   <si>
@@ -217,9 +169,6 @@
     <t>chili powder</t>
   </si>
   <si>
-    <t>clove garlic</t>
-  </si>
-  <si>
     <t>ginger</t>
   </si>
   <si>
@@ -229,9 +178,6 @@
     <t>green pepper</t>
   </si>
   <si>
-    <t>ground cinnamon</t>
-  </si>
-  <si>
     <t>heavy cream</t>
   </si>
   <si>
@@ -259,16 +205,28 @@
     <t>red pepper</t>
   </si>
   <si>
-    <t>shortening</t>
-  </si>
-  <si>
     <t>tomato sauce</t>
   </si>
   <si>
-    <t>basic</t>
-  </si>
-  <si>
-    <t>X</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>contains_meat</t>
+  </si>
+  <si>
+    <t>contains_nuts</t>
+  </si>
+  <si>
+    <t>contains_dairy</t>
+  </si>
+  <si>
+    <t>contains_eggs</t>
+  </si>
+  <si>
+    <t>contains_soy</t>
+  </si>
+  <si>
+    <t>contains_gluten</t>
   </si>
 </sst>
 </file>
@@ -279,21 +237,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -301,7 +259,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -309,7 +267,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -317,35 +275,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -353,7 +311,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -361,14 +319,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -376,14 +334,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -391,7 +349,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -399,14 +357,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -756,48 +714,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - הדגשה1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - הדגשה2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - הדגשה3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - הדגשה4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - הדגשה5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - הדגשה6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - הדגשה1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - הדגשה2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - הדגשה3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - הדגשה4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - הדגשה5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - הדגשה6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - הדגשה1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - הדגשה2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - הדגשה3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - הדגשה4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - הדגשה5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - הדגשה6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="הדגשה1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="הדגשה2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="הדגשה3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="הדגשה4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="הדגשה5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="הדגשה6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="הערה" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="חישוב" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="טוב" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="טקסט אזהרה" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="טקסט הסברי" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="כותרת" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="כותרת 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="כותרת 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="כותרת 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="כותרת 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="ניטראלי" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="סה&quot;כ" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="פלט" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="קלט" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="רע" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="תא מסומן" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="תא מקושר" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -813,30 +771,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:K76" totalsRowShown="0">
-  <autoFilter ref="A1:K76" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A50">
-    <sortCondition ref="A1:A50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H62" totalsRowShown="0">
+  <autoFilter ref="A1:H62" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A43">
+    <sortCondition ref="A1:A43"/>
   </sortState>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="grocery"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="price"/>
-    <tableColumn id="12" xr3:uid="{DA7DD15B-014C-42BB-A42C-A088881776E6}" name="basic"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="meat"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="fish"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="honey"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="nuts"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="eggs"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="milk"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="soy"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="wheat"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="contains_meat"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="contains_nuts"/>
+    <tableColumn id="4" xr3:uid="{E165D503-0F26-47DF-81D3-E5C3C8E13485}" name="contains_dairy"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="contains_eggs"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="contains_soy"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="contains_gluten"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1132,345 +1087,336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K76"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.31640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>50</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="B6">
+        <v>18</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="B7">
-        <v>18</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="B8">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="B9">
-        <v>7</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="B10">
-        <v>10</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B11">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="B12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13">
         <v>25</v>
       </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="B14">
-        <v>25</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="B15">
         <v>40</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="B16">
         <v>40</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B17">
-        <v>40</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="B20">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B22">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="B23">
-        <v>6</v>
-      </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B24">
         <v>12</v>
       </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="B25">
-        <v>5</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B26">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="B27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="B28">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B29">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="B30">
-        <v>45</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A31" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="B31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="B32">
-        <v>20</v>
-      </c>
-      <c r="I32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B33">
         <v>20</v>
@@ -1479,23 +1425,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="B34">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A35" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="B35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1503,357 +1452,240 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="B37">
+        <v>12</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38">
         <v>20</v>
       </c>
-      <c r="H37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38">
-        <v>10</v>
-      </c>
-      <c r="I38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="B39">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="B40">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A42" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43">
+        <v>30</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45">
+        <v>25</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>72</v>
-      </c>
-      <c r="B41">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A50" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A52" t="s">
         <v>12</v>
       </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42">
-        <v>20</v>
-      </c>
-      <c r="G42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>53</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>30</v>
-      </c>
-      <c r="C45" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>8</v>
-      </c>
-      <c r="B46">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>73</v>
-      </c>
-      <c r="B47">
+      <c r="B52">
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>58</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>74</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>49</v>
-      </c>
-      <c r="B50">
-        <v>30</v>
-      </c>
-      <c r="I50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>48</v>
-      </c>
-      <c r="B51">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A53" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53">
+        <v>15</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A54" t="s">
         <v>29</v>
-      </c>
-      <c r="B52">
-        <v>25</v>
-      </c>
-      <c r="G52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>39</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>36</v>
       </c>
       <c r="B54">
         <v>20</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A55" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="B55">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A56" t="s">
+        <v>32</v>
+      </c>
+      <c r="B56">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>75</v>
-      </c>
-      <c r="B56">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B57">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A58" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="B58">
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A59" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="B59">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A60" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B60">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A61" t="s">
-        <v>10</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="B61">
+        <v>30</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A62" t="s">
-        <v>79</v>
-      </c>
-      <c r="C62" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
         <v>4</v>
       </c>
-      <c r="C63" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>23</v>
-      </c>
-      <c r="B64">
-        <v>15</v>
-      </c>
-      <c r="I64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>41</v>
-      </c>
-      <c r="B65">
-        <v>20</v>
-      </c>
-      <c r="J65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>3</v>
-      </c>
-      <c r="B66">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>44</v>
-      </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>80</v>
-      </c>
-      <c r="B68">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>33</v>
-      </c>
-      <c r="B69">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>38</v>
-      </c>
-      <c r="C70" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>52</v>
-      </c>
-      <c r="B71">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>51</v>
-      </c>
-      <c r="C72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>13</v>
-      </c>
-      <c r="B73">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>28</v>
-      </c>
-      <c r="B74">
-        <v>30</v>
-      </c>
-      <c r="G74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>19</v>
-      </c>
-      <c r="C75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>6</v>
-      </c>
-      <c r="B76">
+      <c r="B62">
         <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ladies and gentlemen we have a db
</commit_message>
<xml_diff>
--- a/backend/datasets/raw_ingredients.xlsx
+++ b/backend/datasets/raw_ingredients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Documents\University\Computer Science\courses\99_misc\hackathon\meal_planner_huji_hackathon\backend\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036ECDC8-B6F0-4CE4-A11C-ED2590F61454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB89300C-F237-4E99-8C18-5A171EC515B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>chicken</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>contains_gluten</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -771,13 +774,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H62" totalsRowShown="0">
-  <autoFilter ref="A1:H62" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I62" totalsRowShown="0">
+  <autoFilter ref="A1:I62" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A43">
     <sortCondition ref="A1:A43"/>
   </sortState>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="name"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id"/>
+    <tableColumn id="5" xr3:uid="{1D2E4D11-D04A-4CD1-87DD-2BDDD974097E}" name="name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="price"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="contains_meat"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="contains_nuts"/>
@@ -1087,597 +1091,784 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="23.31640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.31640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>63</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>64</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>67</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>40</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>50</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>43</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>44</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>18</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A7" t="s">
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A9" t="s">
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>45</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>10</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A10" t="s">
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>39</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A11" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>38</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A12" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>25</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A13" t="s">
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>46</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>25</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A14" t="s">
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>0</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>40</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A15" t="s">
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>47</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>40</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A16" t="s">
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>27</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>40</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A17" t="s">
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>48</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A18" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>28</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A19" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>13</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A20" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>31</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A21" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>21</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>6</v>
       </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A22" t="s">
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>14</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>12</v>
       </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A23" t="s">
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>2</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>5</v>
       </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A24" t="s">
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>30</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A25" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>49</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A26" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>50</v>
       </c>
-      <c r="B26">
+      <c r="C26">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A27" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>51</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A28" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>41</v>
       </c>
-      <c r="B28">
+      <c r="C28">
         <v>45</v>
       </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A29" t="s">
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>52</v>
       </c>
-      <c r="B29">
+      <c r="C29">
         <v>20</v>
       </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A30" t="s">
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
         <v>11</v>
       </c>
-      <c r="B30">
+      <c r="C30">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A31" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
         <v>53</v>
       </c>
-      <c r="B31">
+      <c r="C31">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A32" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
         <v>6</v>
       </c>
-      <c r="B32">
+      <c r="C32">
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A33" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>10</v>
       </c>
-      <c r="B33">
+      <c r="C33">
         <v>20</v>
       </c>
-      <c r="F33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A34" t="s">
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
         <v>15</v>
       </c>
-      <c r="B34">
+      <c r="C34">
         <v>10</v>
       </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A35" t="s">
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
         <v>24</v>
       </c>
-      <c r="B35">
+      <c r="C35">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A36" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
         <v>9</v>
       </c>
-      <c r="B36">
+      <c r="C36">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A37" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
         <v>54</v>
       </c>
-      <c r="B37">
+      <c r="C37">
         <v>12</v>
       </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A38" t="s">
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
         <v>18</v>
       </c>
-      <c r="B38">
+      <c r="C38">
         <v>20</v>
       </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A39" t="s">
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
         <v>5</v>
       </c>
-      <c r="B39">
+      <c r="C39">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A40" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
         <v>55</v>
       </c>
-      <c r="B40">
+      <c r="C40">
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A41" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
         <v>42</v>
       </c>
-      <c r="B41">
+      <c r="C41">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A42" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
         <v>56</v>
       </c>
-      <c r="B42">
+      <c r="C42">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A43" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
         <v>36</v>
       </c>
-      <c r="B43">
+      <c r="C43">
         <v>30</v>
       </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A44" t="s">
+      <c r="F43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
         <v>35</v>
       </c>
-      <c r="B44">
+      <c r="C44">
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A45" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
         <v>20</v>
       </c>
-      <c r="B45">
+      <c r="C45">
         <v>25</v>
       </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A46" t="s">
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
         <v>26</v>
       </c>
-      <c r="B46">
+      <c r="C46">
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A47" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
         <v>34</v>
       </c>
-      <c r="B47">
+      <c r="C47">
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.75">
-      <c r="A48" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
         <v>57</v>
       </c>
-      <c r="B48">
+      <c r="C48">
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A49" t="s">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
         <v>58</v>
       </c>
-      <c r="B49">
+      <c r="C49">
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A50" t="s">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
         <v>59</v>
       </c>
-      <c r="B50">
+      <c r="C50">
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A51" t="s">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
         <v>60</v>
       </c>
-      <c r="B51">
+      <c r="C51">
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A52" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
         <v>12</v>
       </c>
-      <c r="B52">
+      <c r="C52">
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A53" t="s">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
         <v>16</v>
       </c>
-      <c r="B53">
+      <c r="C53">
         <v>15</v>
       </c>
-      <c r="E53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A54" t="s">
+      <c r="F53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
         <v>29</v>
       </c>
-      <c r="B54">
+      <c r="C54">
         <v>20</v>
       </c>
-      <c r="G54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A55" t="s">
+      <c r="H54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
         <v>3</v>
       </c>
-      <c r="B55">
+      <c r="C55">
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A56" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
         <v>32</v>
       </c>
-      <c r="B56">
+      <c r="C56">
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A57" t="s">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
         <v>61</v>
       </c>
-      <c r="B57">
+      <c r="C57">
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A58" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
         <v>23</v>
       </c>
-      <c r="B58">
+      <c r="C58">
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A59" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
         <v>37</v>
       </c>
-      <c r="B59">
+      <c r="C59">
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A60" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
         <v>8</v>
       </c>
-      <c r="B60">
+      <c r="C60">
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A61" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
         <v>19</v>
       </c>
-      <c r="B61">
+      <c r="C61">
         <v>30</v>
       </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A62" t="s">
+      <c r="E61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
         <v>4</v>
       </c>
-      <c r="B62">
+      <c r="C62">
         <v>35</v>
       </c>
     </row>

</xml_diff>